<commit_message>
Testing Defect Report Updated
</commit_message>
<xml_diff>
--- a/Calendar Module/Defect Report/Calendar_Module_Defects.xlsx
+++ b/Calendar Module/Defect Report/Calendar_Module_Defects.xlsx
@@ -83,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -118,13 +118,6 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -196,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,34 +216,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -331,10 +296,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:R62"/>
+  <dimension ref="A2:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -608,280 +573,49 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="9"/>
-      <c r="E25" s="6"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="10"/>
-      <c r="E26" s="6"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="10"/>
-      <c r="E27" s="6"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="10"/>
-      <c r="E28" s="6"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="6"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="11"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="6"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="11"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="6"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="13"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="8"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="6"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="2">
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="A5:N5"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A62:J62"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -901,7 +635,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -928,7 +662,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>